<commit_message>
Dropdown code completed. couldnot run.
</commit_message>
<xml_diff>
--- a/TrainerManagementSystem/src/main/resources/SignupExcel.xlsx
+++ b/TrainerManagementSystem/src/main/resources/SignupExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\testing\TMSNew\ICTAK\TrainerManagementSystem\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0F57BD-27D7-43AB-9708-3EE5FD0C8A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AD5343-A551-4B8C-B817-FBE76F1418C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,21 @@
   </si>
   <si>
     <t>Abc@1234</t>
+  </si>
+  <si>
+    <t>Full Stack Development </t>
+  </si>
+  <si>
+    <t>Data Science &amp; Analytics </t>
+  </si>
+  <si>
+    <t>Cyber Security Analyst </t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>Robotic Process Automation</t>
   </si>
 </sst>
 </file>
@@ -407,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -418,7 +433,7 @@
     <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,8 +464,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -480,6 +498,24 @@
       </c>
       <c r="J3" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>